<commit_message>
catching up on weeks 5,6,7
</commit_message>
<xml_diff>
--- a/data/Player_images_S49_Survivor.xlsx
+++ b/data/Player_images_S49_Survivor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IsaacSchultz\Documents\Survivor_Python\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72C67C3D-2937-4F43-9374-9D8235F6521F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F498B26E-B8DE-4EBB-9AB3-7F56C32840E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{689D6602-70B1-45F1-BB5C-109A2BB84EA3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{689D6602-70B1-45F1-BB5C-109A2BB84EA3}"/>
   </bookViews>
   <sheets>
     <sheet name="Images" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>Player</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Week 4</t>
+  </si>
+  <si>
+    <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>Week 7</t>
   </si>
 </sst>
 </file>
@@ -1037,17 +1046,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A6BF08F-3346-4A5B-8A4A-50292AB38C8D}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="200.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="200.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1061,7 +1070,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1072,7 +1081,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1086,7 +1095,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1100,18 +1109,21 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
       <c r="D5">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1122,7 +1134,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1136,7 +1148,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -1147,7 +1159,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1161,7 +1173,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -1172,18 +1184,21 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
       </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
       <c r="D11">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -1197,7 +1212,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1208,7 +1223,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1219,7 +1234,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1230,18 +1245,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>32</v>
       </c>
       <c r="B16" t="s">
         <v>33</v>
       </c>
+      <c r="C16" t="s">
+        <v>25</v>
+      </c>
       <c r="D16">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1252,7 +1270,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1263,7 +1281,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1281,15 +1299,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08C3063B-C826-4B08-85BF-C9C7D8FD5FC4}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>40</v>
       </c>
@@ -1297,7 +1315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>41</v>
       </c>
@@ -1305,7 +1323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -1313,7 +1331,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>43</v>
       </c>
@@ -1321,7 +1339,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1329,12 +1347,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>46</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>